<commit_message>
updated files that were missing zmin, zmax
</commit_message>
<xml_diff>
--- a/psidis/expdata/20000.xlsx
+++ b/psidis/expdata/20000.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10709"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="11012"/>
   <workbookPr autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jacobethier/Documents/fitpack/database/psidis/expdata/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/fafd12/GIT/fitpack2/database/psidis/expdata/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8B9B20C9-BEA4-C94A-BE2B-F93726DB6A43}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B207CC90-D997-ED49-9377-BD6E15B133CF}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3220" yWindow="6880" windowWidth="24560" windowHeight="13180" tabRatio="979" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="440" yWindow="520" windowWidth="16400" windowHeight="10280" tabRatio="979" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="140001" iterateDelta="1E-4"/>
+  <calcPr calcId="140001"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="15">
   <si>
     <t>X</t>
   </si>
@@ -64,6 +64,12 @@
   </si>
   <si>
     <t>SMC</t>
+  </si>
+  <si>
+    <t>zmin</t>
+  </si>
+  <si>
+    <t>zmax</t>
   </si>
 </sst>
 </file>
@@ -475,10 +481,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I13"/>
+  <dimension ref="A1:K13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J7" sqref="J7"/>
+      <selection activeCell="L11" sqref="L11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -486,7 +492,7 @@
     <col min="1" max="8" width="8.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -514,8 +520,14 @@
       <c r="I1" s="1" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A2" s="1">
         <v>5.0000000000000001E-3</v>
       </c>
@@ -543,8 +555,14 @@
       <c r="I2" s="1" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J2">
+        <v>0.2</v>
+      </c>
+      <c r="K2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A3" s="1">
         <v>8.0000000000000002E-3</v>
       </c>
@@ -572,8 +590,14 @@
       <c r="I3" s="1" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J3">
+        <v>0.2</v>
+      </c>
+      <c r="K3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A4" s="1">
         <v>1.4E-2</v>
       </c>
@@ -601,8 +625,14 @@
       <c r="I4" s="1" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J4">
+        <v>0.2</v>
+      </c>
+      <c r="K4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A5" s="1">
         <v>2.5000000000000001E-2</v>
       </c>
@@ -630,8 +660,14 @@
       <c r="I5" s="1" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J5">
+        <v>0.2</v>
+      </c>
+      <c r="K5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A6" s="1">
         <v>3.5000000000000003E-2</v>
       </c>
@@ -659,8 +695,14 @@
       <c r="I6" s="1" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J6">
+        <v>0.2</v>
+      </c>
+      <c r="K6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A7" s="1">
         <v>4.9000000000000002E-2</v>
       </c>
@@ -688,8 +730,14 @@
       <c r="I7" s="1" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J7">
+        <v>0.2</v>
+      </c>
+      <c r="K7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A8" s="1">
         <v>7.6999999999999999E-2</v>
       </c>
@@ -717,8 +765,14 @@
       <c r="I8" s="1" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J8">
+        <v>0.2</v>
+      </c>
+      <c r="K8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A9" s="1">
         <v>0.122</v>
       </c>
@@ -746,8 +800,14 @@
       <c r="I9" s="1" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J9">
+        <v>0.2</v>
+      </c>
+      <c r="K9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A10" s="1">
         <v>0.17299999999999999</v>
       </c>
@@ -775,8 +835,14 @@
       <c r="I10" s="1" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J10">
+        <v>0.2</v>
+      </c>
+      <c r="K10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A11" s="1">
         <v>0.24199999999999999</v>
       </c>
@@ -804,8 +870,14 @@
       <c r="I11" s="1" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J11">
+        <v>0.2</v>
+      </c>
+      <c r="K11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A12" s="1">
         <v>0.34200000000000003</v>
       </c>
@@ -833,8 +905,14 @@
       <c r="I12" s="1" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J12">
+        <v>0.2</v>
+      </c>
+      <c r="K12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A13" s="1">
         <v>0.48</v>
       </c>
@@ -861,6 +939,12 @@
       </c>
       <c r="I13" s="1" t="s">
         <v>12</v>
+      </c>
+      <c r="J13">
+        <v>0.2</v>
+      </c>
+      <c r="K13">
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>